<commit_message>
Added the script to LoginPageTest to test the Invalid entries in OTP field.
</commit_message>
<xml_diff>
--- a/src/test/resources/eazypayoutTestData.xlsx
+++ b/src/test/resources/eazypayoutTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Phedora\Eazypayouts\Eazypayout Automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5BA47E-207B-46F3-9F6A-F3140EE62DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92458C5D-C85F-464F-8EB8-3DB4B95CE983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>mobile num</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>!@#$%^&amp;*()</t>
+  </si>
+  <si>
+    <t>OTP field</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>!@#$%^</t>
   </si>
 </sst>
 </file>
@@ -96,12 +105,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -383,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,10 +406,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -426,10 +436,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -445,7 +455,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -457,6 +467,34 @@
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>897048652</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3">
+        <v>456789</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>4567891</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>45678</v>
       </c>
     </row>
   </sheetData>
@@ -466,6 +504,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{BADA2CE0-5D8C-4D63-8107-424C202C25BD}"/>
+    <hyperlink ref="B16" r:id="rId2" xr:uid="{0480FDF7-D707-4DF2-9A0F-26283A134E1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>